<commit_message>
resumen de reporte agregado
</commit_message>
<xml_diff>
--- a/public/Visitas.xlsx
+++ b/public/Visitas.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Visistas" sheetId="1" r:id="rId1"/>
+    <sheet name="resumen hogares" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -506,4 +507,98 @@
     <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Id_hogar</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Edad_promedio</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Genero</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Nivel_educacional</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Estado_civil</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Nacionalidad</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>46</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rutas exportacion de datos arreglada
</commit_message>
<xml_diff>
--- a/public/Visitas.xlsx
+++ b/public/Visitas.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,7 +464,7 @@
         <v>completo</v>
       </c>
       <c r="D3" s="1">
-        <v>45089.99947916667</v>
+        <v>45087.99947916667</v>
       </c>
       <c r="E3">
         <v>222</v>
@@ -473,7 +473,7 @@
         <v>35</v>
       </c>
       <c r="G3" t="str">
-        <v>morande 924</v>
+        <v>serrano 1620</v>
       </c>
       <c r="H3" t="str">
         <v>santiago</v>
@@ -502,79 +502,9 @@
         <v>providencia</v>
       </c>
     </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">carrete_x000d_
-</v>
-      </c>
-      <c r="C5" t="str">
-        <v>incompleto</v>
-      </c>
-      <c r="E5">
-        <v>11232313</v>
-      </c>
-      <c r="F5">
-        <v>37</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Carrion 1346</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Independencia</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6" t="str">
-        <v>otro carrete</v>
-      </c>
-      <c r="C6" t="str">
-        <v>incompleto</v>
-      </c>
-      <c r="E6">
-        <v>2049652</v>
-      </c>
-      <c r="F6">
-        <v>37</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Carrion 1346</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Independencia</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Carencia alimentos</v>
-      </c>
-      <c r="C7" t="str">
-        <v>incompleto</v>
-      </c>
-      <c r="E7">
-        <v>222</v>
-      </c>
-      <c r="F7">
-        <v>39</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Nueva de Matte 2580</v>
-      </c>
-      <c r="H7" t="str">
-        <v>Independencia</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>